<commit_message>
Committing the flow pattern
</commit_message>
<xml_diff>
--- a/Data Files/POS-TestData.xlsx
+++ b/Data Files/POS-TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csharmila\Documents\UiPath\POS-TestAutomationProject\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csharmila\Documents\UiPath\POSCUI\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,9 +102,6 @@
     <t>Tilak</t>
   </si>
   <si>
-    <t>Sale/Return</t>
-  </si>
-  <si>
     <t>Sale</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
     <t>Complete the return successfully and return to main menu
 If salesperson ID is incorrect, capture error and return to main screen
 If customer is not available, capture error and return to main screen</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -551,7 +553,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -566,13 +568,13 @@
         <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>1</v>
@@ -593,13 +595,13 @@
         <v>16</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
@@ -607,7 +609,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="6">
         <v>5649</v>
@@ -641,19 +643,19 @@
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6">
         <v>5649</v>
@@ -671,7 +673,7 @@
         <v>1234</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="6">
         <v>44333</v>
@@ -692,22 +694,22 @@
         <v>5</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="C4" s="6">
         <v>5649</v>
@@ -732,18 +734,18 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="6">
         <v>5649</v>
@@ -768,18 +770,18 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6">
         <v>5649</v>
@@ -797,7 +799,7 @@
         <v>1234</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="6">
         <v>44333</v>
@@ -819,19 +821,19 @@
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="6">
         <v>5649</v>
@@ -849,7 +851,7 @@
         <v>1234</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="6">
         <v>44333</v>
@@ -864,10 +866,10 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Return Scenarios Update - Commit
</commit_message>
<xml_diff>
--- a/Data Files/POS-TestData.xlsx
+++ b/Data Files/POS-TestData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
   <si>
     <t>SalesPerson</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>Sale with Cash - ESP and Promo Code</t>
-  </si>
-  <si>
-    <t>B5550000001011</t>
   </si>
   <si>
     <t>Complete the Sale successfully and return to main menu
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>ABZZ0000001019</t>
   </si>
 </sst>
 </file>
@@ -536,9 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -553,7 +551,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -568,13 +566,13 @@
         <v>13</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>1</v>
@@ -595,10 +593,10 @@
         <v>16</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>26</v>
@@ -643,19 +641,19 @@
       </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6">
         <v>5649</v>
@@ -667,49 +665,31 @@
         <v>9</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1234</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="6">
-        <v>44333</v>
-      </c>
-      <c r="J3" s="6">
-        <v>200181600</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="R3" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C4" s="6">
         <v>5649</v>
@@ -734,18 +714,18 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6">
         <v>5649</v>
@@ -760,25 +740,37 @@
         <v>5</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="J5" s="6">
+        <v>200181600</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="8"/>
       <c r="R5" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>25</v>
@@ -799,7 +791,7 @@
         <v>1234</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="6">
         <v>44333</v>
@@ -821,19 +813,19 @@
       </c>
       <c r="O6" s="8"/>
       <c r="P6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6">
         <v>5649</v>
@@ -851,7 +843,7 @@
         <v>1234</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="6">
         <v>44333</v>
@@ -866,10 +858,10 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues with slip receipt and Diamond Bond and ESP
</commit_message>
<xml_diff>
--- a/Data Files/POS-TestData.xlsx
+++ b/Data Files/POS-TestData.xlsx
@@ -684,12 +684,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6">
         <v>5649</v>
@@ -704,28 +704,40 @@
         <v>5</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6" t="s">
-        <v>34</v>
-      </c>
+      <c r="J4" s="6">
+        <v>200181600</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="8"/>
       <c r="R4" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C5" s="6">
         <v>5649</v>
@@ -740,32 +752,20 @@
         <v>5</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="6">
-        <v>200181600</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="8"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="R5" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">

</xml_diff>